<commit_message>
fix se arreglo bug en la funcion calcular fechas de matricula ya que si no existia dias de duracion de curso esto traia un inf o nan como error
</commit_message>
<xml_diff>
--- a/temp_files/validacion_inicial.xlsx
+++ b/temp_files/validacion_inicial.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +589,41 @@
           <t>CourseDaysDuration</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>timestart</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>timeend</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>NRO_DIAS_DE_MATRICULAS</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>El tiempo de matricula es invalido</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Numero_Wapp_Incorrecto</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Numero_Con_Prefijo</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>El campo del pais esta vacío</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -615,9 +650,7 @@
           <t>COLOMBIA</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>3209006290</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>Universal Learning</t>
@@ -707,9 +740,32 @@
       <c r="AD2" t="n">
         <v>7</v>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>25</t>
+      <c r="AE2" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1727686800</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -831,6 +887,35 @@
       </c>
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>+5732090wr0{6290a</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -955,9 +1040,36 @@
       <c r="AD4" t="n">
         <v>4</v>
       </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>7</t>
+      <c r="AE4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>1726131600</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>+573209006290</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1084,9 +1196,36 @@
       <c r="AD5" t="n">
         <v>4</v>
       </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>7</t>
+      <c r="AE5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1726131600</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>+573209006290</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1209,9 +1348,36 @@
       <c r="AD6" t="n">
         <v>7</v>
       </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>25</t>
+      <c r="AE6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>1726131600</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>+573183812254</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -1332,9 +1498,36 @@
       <c r="AD7" t="n">
         <v>7</v>
       </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>25</t>
+      <c r="AE7" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1725526800</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1727686800</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>+573183812254</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>

</xml_diff>